<commit_message>
Counts yes and no values
Counts yes and no values
</commit_message>
<xml_diff>
--- a/rule extaction with cp-nets/Rules extracted from DT.xlsx
+++ b/rule extaction with cp-nets/Rules extracted from DT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
   <si>
     <t>Dtree Path</t>
   </si>
@@ -612,6 +612,12 @@
   </si>
   <si>
     <t>td &gt; 692, pn = "Agriculture", at &gt; 41, os3 &gt;= 41, os4 &lt;= 123, ssc &lt;= 772, os5 &lt;=133, os6 &lt;=136</t>
+  </si>
+  <si>
+    <t>td&gt;=705</t>
+  </si>
+  <si>
+    <t>Revised</t>
   </si>
 </sst>
 </file>
@@ -2100,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,7 +2118,7 @@
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -2122,8 +2128,11 @@
       <c r="D1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2133,9 +2142,12 @@
       <c r="D2" s="28" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2146,8 +2158,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2158,8 +2170,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:4" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2170,8 +2182,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2182,8 +2194,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:4" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2194,8 +2206,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:4" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2206,8 +2218,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:4" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
To measure Performance of Agriculture data
To measure Performance of Agriculture data
</commit_message>
<xml_diff>
--- a/rule extaction with cp-nets/Rules extracted from DT.xlsx
+++ b/rule extaction with cp-nets/Rules extracted from DT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="168">
   <si>
     <t>Dtree Path</t>
   </si>
@@ -618,6 +618,9 @@
   </si>
   <si>
     <t>Revised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label </t>
   </si>
 </sst>
 </file>
@@ -2106,19 +2109,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -2126,179 +2129,182 @@
         <v>134</v>
       </c>
       <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
         <v>163</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="E4" s="28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="E8" s="29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="29" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="E12" s="29" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="E14" s="29" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="167.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="E16" s="29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:4" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:5" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="29" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:5" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="E20" s="29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" ht="129" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="E22" s="29" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:4" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:5" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="E24" s="29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="E26" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>